<commit_message>
Testing beginners selection v3
</commit_message>
<xml_diff>
--- a/NTDS_Groningen.xlsx
+++ b/NTDS_Groningen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6000" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="7800" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>